<commit_message>
Conditional formatting now leaves the untouched formats alone. Issue 8053
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/ConditionalFormatting/CFColorScaleLowHigh.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/ConditionalFormatting/CFColorScaleLowHigh.xlsx
@@ -74,36 +74,11 @@
   </x:cellStyles>
   <x:dxfs count="1">
     <x:dxf>
-      <x:font>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="11"/>
-        <x:color rgb="FF000000"/>
-        <x:name val="Calibri"/>
-        <x:family val="2"/>
-      </x:font>
+      <x:font/>
       <x:fill>
-        <x:patternFill patternType="none">
-          <x:fgColor indexed="64"/>
-          <x:bgColor indexed="64"/>
-        </x:patternFill>
+        <x:patternFill/>
       </x:fill>
-      <x:border diagonalUp="0" diagonalDown="0">
-        <x:left style="none">
-          <x:color rgb="FF000000"/>
-        </x:left>
-        <x:right style="none">
-          <x:color rgb="FF000000"/>
-        </x:right>
-        <x:top style="none">
-          <x:color rgb="FF000000"/>
-        </x:top>
-        <x:bottom style="none">
-          <x:color rgb="FF000000"/>
-        </x:bottom>
-        <x:diagonal style="none">
-          <x:color rgb="FF000000"/>
-        </x:diagonal>
-      </x:border>
+      <x:border/>
     </x:dxf>
   </x:dxfs>
 </x:styleSheet>

</xml_diff>

<commit_message>
Fixed issue when modifying a range with conditional formats. Added more formulas.
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/ConditionalFormatting/CFColorScaleLowHigh.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/ConditionalFormatting/CFColorScaleLowHigh.xlsx
@@ -83,7 +83,9 @@
     <x:dxf>
       <x:font/>
       <x:fill>
-        <x:patternFill/>
+        <x:patternFill>
+          <x:bgColor indexed="64"/>
+        </x:patternFill>
       </x:fill>
       <x:border/>
     </x:dxf>

</xml_diff>

<commit_message>
Fixed the fix on deleting cells with conditional formatting.
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/ConditionalFormatting/CFColorScaleLowHigh.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/ConditionalFormatting/CFColorScaleLowHigh.xlsx
@@ -83,9 +83,7 @@
     <x:dxf>
       <x:font/>
       <x:fill>
-        <x:patternFill>
-          <x:bgColor indexed="64"/>
-        </x:patternFill>
+        <x:patternFill/>
       </x:fill>
       <x:border/>
     </x:dxf>

</xml_diff>